<commit_message>
updated test input file
</commit_message>
<xml_diff>
--- a/tests/input_file/inputparameters.xlsx
+++ b/tests/input_file/inputparameters.xlsx
@@ -4413,7 +4413,7 @@
   <dimension ref="A1:AK1895"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5294,7 +5294,7 @@
         <v>41</v>
       </c>
       <c r="D16" s="8">
-        <v>0.43852951083798603</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="8">
         <v>0.27896020164795099</v>

</xml_diff>